<commit_message>
Ticket and Payment integration with front end.
</commit_message>
<xml_diff>
--- a/Progress Tracker.xlsx
+++ b/Progress Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\School\SWE M.Eng\ENSF 614\Project\Flight-Reservation-Web-Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F79AF2D-D715-4A7D-8FE0-C1F7B46F1A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D463D3-1814-4DC5-848E-455AB34A8C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{A167CAB8-BBBC-417B-88FD-FE2CA15B1842}"/>
+    <workbookView xWindow="28680" yWindow="-5625" windowWidth="38640" windowHeight="21120" xr2:uid="{A167CAB8-BBBC-417B-88FD-FE2CA15B1842}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric-I" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>Task</t>
   </si>
@@ -307,10 +307,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -628,19 +628,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7141C6-0680-45AE-AA39-E8A3A429789B}">
   <dimension ref="B2:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="54.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.23046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.3046875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
@@ -657,7 +657,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="13" t="s">
         <v>3</v>
       </c>
@@ -673,7 +673,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
         <v>4</v>
       </c>
@@ -689,7 +689,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="13" t="s">
         <v>6</v>
       </c>
@@ -705,7 +705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="13" t="s">
         <v>5</v>
       </c>
@@ -713,13 +713,15 @@
         <v>4</v>
       </c>
       <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
+      <c r="E6" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="F6" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="13" t="s">
         <v>7</v>
       </c>
@@ -727,13 +729,15 @@
         <v>4</v>
       </c>
       <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
+      <c r="E7" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="F7" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="13" t="s">
         <v>8</v>
       </c>
@@ -741,13 +745,15 @@
         <v>4</v>
       </c>
       <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
+      <c r="E8" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="F8" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="13" t="s">
         <v>9</v>
       </c>
@@ -755,13 +761,15 @@
         <v>5</v>
       </c>
       <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
+      <c r="E9" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="F9" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="13" t="s">
         <v>10</v>
       </c>
@@ -775,7 +783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="13" t="s">
         <v>11</v>
       </c>
@@ -789,7 +797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="13" t="s">
         <v>12</v>
       </c>
@@ -797,13 +805,15 @@
         <v>2</v>
       </c>
       <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
+      <c r="E12" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="F12" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="13" t="s">
         <v>13</v>
       </c>
@@ -817,7 +827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="13" t="s">
         <v>14</v>
       </c>
@@ -833,7 +843,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="13" t="s">
         <v>15</v>
       </c>
@@ -847,7 +857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="13" t="s">
         <v>16</v>
       </c>
@@ -861,7 +871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="13" t="s">
         <v>18</v>
       </c>
@@ -875,7 +885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="13" t="s">
         <v>17</v>
       </c>
@@ -891,7 +901,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B19" s="15" t="s">
         <v>48</v>
       </c>
@@ -906,7 +916,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="1">
         <f>SUM(F3:F18)</f>
-        <v>27</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -923,16 +933,16 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="36.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.21875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="3.5546875" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.84375" style="6"/>
+    <col min="2" max="2" width="36.69140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.23046875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="3.53515625" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="8.84375" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="16" t="s">
         <v>22</v>
       </c>
@@ -943,111 +953,111 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="19" t="s">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B3" s="22" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="21"/>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="19"/>
+      <c r="D3" s="19"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="22"/>
       <c r="C4" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="21"/>
-    </row>
-    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="B5" s="19"/>
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="2:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="B5" s="22"/>
       <c r="C5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="21"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="19"/>
+      <c r="D5" s="19"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="22"/>
       <c r="C6" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="21"/>
-    </row>
-    <row r="7" spans="2:4" ht="60" x14ac:dyDescent="0.2">
-      <c r="B7" s="19" t="s">
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" spans="2:4" ht="62" x14ac:dyDescent="0.35">
+      <c r="B7" s="22" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="21"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="19"/>
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="22"/>
       <c r="C8" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="21"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="19"/>
+      <c r="D8" s="19"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="22"/>
       <c r="C9" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="21"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="19"/>
+      <c r="D9" s="19"/>
+    </row>
+    <row r="10" spans="2:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="B10" s="22"/>
       <c r="C10" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="21"/>
-    </row>
-    <row r="11" spans="2:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="B11" s="19"/>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="2:4" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="B11" s="22"/>
       <c r="C11" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="21"/>
-    </row>
-    <row r="12" spans="2:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="B12" s="19"/>
+      <c r="D11" s="19"/>
+    </row>
+    <row r="12" spans="2:4" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="B12" s="22"/>
       <c r="C12" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="21"/>
-    </row>
-    <row r="13" spans="2:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="B13" s="19"/>
+      <c r="D12" s="19"/>
+    </row>
+    <row r="13" spans="2:4" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="22"/>
       <c r="C13" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="21"/>
-    </row>
-    <row r="14" spans="2:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="B14" s="22" t="s">
+      <c r="D13" s="19"/>
+    </row>
+    <row r="14" spans="2:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="B14" s="21" t="s">
         <v>42</v>
       </c>
       <c r="C14" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="21"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="19" t="s">
+      <c r="D14" s="19"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B15" s="22" t="s">
         <v>45</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="21"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="19"/>
+      <c r="D15" s="19"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B16" s="22"/>
       <c r="C16" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="21"/>
+      <c r="D16" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1063,19 +1073,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84CE03EF-6F19-401E-8CA5-0882123B7144}">
   <dimension ref="B2:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="8.84375" style="5"/>
     <col min="2" max="2" width="71" style="7" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="5"/>
+    <col min="3" max="3" width="12.3046875" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="8.84375" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1083,47 +1093,47 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" ht="31" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" ht="31" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" ht="31" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B9" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B10" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="2:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Final improvements (mainly to UI).
</commit_message>
<xml_diff>
--- a/Progress Tracker.xlsx
+++ b/Progress Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\School\SWE M.Eng\ENSF 614\Project\Flight-Reservation-Web-Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8472D086-EED4-4DA5-9F04-3CC65BB8E315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD68CB92-286E-49F5-B88E-7CF875ED5C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5625" windowWidth="38640" windowHeight="21120" xr2:uid="{A167CAB8-BBBC-417B-88FD-FE2CA15B1842}"/>
+    <workbookView xWindow="28695" yWindow="-5505" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{A167CAB8-BBBC-417B-88FD-FE2CA15B1842}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric-I" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
   <si>
     <t>Task</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>Allow the system admin to sign in from the system admin page. To save time, we can just have one set of credentials to access the dashboard.</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -628,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7141C6-0680-45AE-AA39-E8A3A429789B}">
   <dimension ref="B2:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -825,10 +828,12 @@
       <c r="D13" s="13">
         <v>5</v>
       </c>
-      <c r="E13" s="14"/>
+      <c r="E13" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="F13" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.35">
@@ -855,10 +860,12 @@
         <v>2</v>
       </c>
       <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
+      <c r="E15" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="F15" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.35">
@@ -869,10 +876,12 @@
         <v>4</v>
       </c>
       <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
+      <c r="E16" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="F16" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
@@ -883,10 +892,12 @@
         <v>4</v>
       </c>
       <c r="D17" s="13"/>
-      <c r="E17" s="14"/>
+      <c r="E17" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="F17" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
@@ -920,7 +931,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="1">
         <f>SUM(F3:F18)</f>
-        <v>50</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -933,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85D5F109-E4C1-403D-9B0D-95963F1EA643}">
   <dimension ref="B2:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -964,28 +975,36 @@
       <c r="C3" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="19"/>
+      <c r="D3" s="19" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4" s="22"/>
       <c r="C4" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="19"/>
+      <c r="D4" s="19" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="5" spans="2:4" ht="31" x14ac:dyDescent="0.35">
       <c r="B5" s="22"/>
       <c r="C5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="19"/>
+      <c r="D5" s="19" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="22"/>
       <c r="C6" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="19"/>
+      <c r="D6" s="19" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="7" spans="2:4" ht="62" x14ac:dyDescent="0.35">
       <c r="B7" s="22" t="s">
@@ -994,49 +1013,63 @@
       <c r="C7" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="19"/>
+      <c r="D7" s="19" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="22"/>
       <c r="C8" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="19"/>
+      <c r="D8" s="19" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="22"/>
       <c r="C9" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="19"/>
+      <c r="D9" s="19" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="10" spans="2:4" ht="31" x14ac:dyDescent="0.35">
       <c r="B10" s="22"/>
       <c r="C10" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="19"/>
+      <c r="D10" s="19" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="11" spans="2:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B11" s="22"/>
       <c r="C11" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="19"/>
+      <c r="D11" s="19" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="12" spans="2:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B12" s="22"/>
       <c r="C12" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="19"/>
+      <c r="D12" s="19" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="13" spans="2:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B13" s="22"/>
       <c r="C13" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="19"/>
+      <c r="D13" s="19" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="14" spans="2:4" ht="31" x14ac:dyDescent="0.35">
       <c r="B14" s="21" t="s">
@@ -1045,7 +1078,9 @@
       <c r="C14" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="19"/>
+      <c r="D14" s="19" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B15" s="22" t="s">
@@ -1054,14 +1089,18 @@
       <c r="C15" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="19"/>
+      <c r="D15" s="19" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" s="22"/>
       <c r="C16" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="19"/>
+      <c r="D16" s="19" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>